<commit_message>
Sync control unit .xlsx with phase 1
</commit_message>
<xml_diff>
--- a/Control Unit.xlsx
+++ b/Control Unit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP\third_Year\first_Semester\computer architecture\project\Five-stages-pipeline-processsor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Third Year\First Term\Computer Architecture\Project\Five-stages-pipeline-processsor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6931B5B2-635E-466D-B3D2-9E56C10E6FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630BC3A0-0CDF-42FE-897F-209F93B7E901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8184" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>Instructio name</t>
   </si>
@@ -114,12 +114,6 @@
     <t>RTI</t>
   </si>
   <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>Interrupt</t>
-  </si>
-  <si>
     <t>00001</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>11010</t>
   </si>
   <si>
-    <t>11011</t>
-  </si>
-  <si>
     <t>CLRC</t>
   </si>
   <si>
@@ -268,6 +259,21 @@
   </si>
   <si>
     <t>CALL</t>
+  </si>
+  <si>
+    <t>MemRead</t>
+  </si>
+  <si>
+    <t>MemWrite</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Will be detected from opcode directly</t>
   </si>
 </sst>
 </file>
@@ -339,16 +345,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,98 +647,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD92692-33F2-46CB-9148-D3ECB8C3F0BA}">
-  <dimension ref="A1:AB29"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="25.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="7" customWidth="1"/>
+    <col min="3" max="29" width="8.88671875" style="3"/>
+    <col min="30" max="30" width="13.77734375" style="3" customWidth="1"/>
+    <col min="31" max="31" width="15" style="3" customWidth="1"/>
+    <col min="32" max="32" width="10.44140625" style="3" customWidth="1"/>
+    <col min="33" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>27</v>
@@ -729,393 +750,624 @@
       <c r="AB1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="AC1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <v>0</v>
-      </c>
-      <c r="P2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>0</v>
-      </c>
-      <c r="R2" s="4">
-        <v>0</v>
-      </c>
-      <c r="S2" s="4">
-        <v>0</v>
-      </c>
-      <c r="T2" s="4">
-        <v>0</v>
-      </c>
-      <c r="U2" s="4">
-        <v>0</v>
-      </c>
-      <c r="V2" s="4">
-        <v>0</v>
-      </c>
-      <c r="W2" s="4">
-        <v>0</v>
-      </c>
-      <c r="X2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>0</v>
-      </c>
-      <c r="R3" s="4">
-        <v>0</v>
-      </c>
-      <c r="S3" s="4">
-        <v>0</v>
-      </c>
-      <c r="T3" s="4">
-        <v>0</v>
-      </c>
-      <c r="U3" s="4">
-        <v>0</v>
-      </c>
-      <c r="V3" s="4">
-        <v>0</v>
-      </c>
-      <c r="W3" s="4">
-        <v>0</v>
-      </c>
-      <c r="X3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="Y10" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="V11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="AF12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="AF13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+      <c r="B22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+      <c r="B23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+      <c r="B24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+      <c r="B25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+      <c r="B26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="O26" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
+      <c r="B27" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P27" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="S28" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A29" s="2"/>
+      <c r="B29" s="6"/>
+      <c r="AC29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC32">
+    <sortCondition ref="B2:B32"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="Q10:T13"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
30 bits control unit phase-3
</commit_message>
<xml_diff>
--- a/Control Unit.xlsx
+++ b/Control Unit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMP\third_Year\first_Semester\computer architecture\project\Five-stages-pipeline-processsor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Third Year\First Term\Computer Architecture\Project\Five-stages-pipeline-processsor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02003470-9B8B-41EB-BED7-CE4FEB89C441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3825A84F-B0DF-4DDE-805B-D76EFB90894E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,23 +424,23 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -727,14 +727,15 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D29" sqref="D29"/>
+      <selection pane="topRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="25.88671875" style="3" customWidth="1"/>
     <col min="2" max="5" width="23.44140625" style="7" customWidth="1"/>
-    <col min="6" max="32" width="8.88671875" style="3"/>
+    <col min="6" max="6" width="9.109375" style="3" customWidth="1"/>
+    <col min="7" max="32" width="8.88671875" style="3"/>
     <col min="33" max="33" width="13.77734375" style="3" customWidth="1"/>
     <col min="34" max="34" width="15" style="3" customWidth="1"/>
     <col min="35" max="35" width="10.44140625" style="3" customWidth="1"/>
@@ -935,7 +936,7 @@
       <c r="C6" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -981,7 +982,7 @@
       <c r="C8" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -1033,12 +1034,12 @@
       <c r="E10" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T10" s="11" t="s">
+      <c r="T10" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
       <c r="AB10" s="10">
         <v>1</v>
       </c>
@@ -1062,10 +1063,10 @@
       <c r="E11" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
       <c r="Y11" s="3">
         <v>1</v>
       </c>
@@ -1089,10 +1090,10 @@
       <c r="E12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
       <c r="AI12" s="10">
         <v>1</v>
       </c>
@@ -1113,10 +1114,10 @@
       <c r="E13" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
       <c r="AI13" s="3">
         <v>1</v>
       </c>
@@ -1398,7 +1399,7 @@
       <c r="D26" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="11" t="s">
         <v>90</v>
       </c>
       <c r="R26" s="10">
@@ -1421,7 +1422,7 @@
       <c r="D27" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="11" t="s">
         <v>90</v>
       </c>
       <c r="S27" s="3">
@@ -1458,40 +1459,40 @@
       <c r="A29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
       <c r="AF29" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.4">
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.4">
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF32">

</xml_diff>